<commit_message>
Changed the longlat of 1114
</commit_message>
<xml_diff>
--- a/data/data_lokasi_rev.xlsx
+++ b/data/data_lokasi_rev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICRAF\Kodingan\icraf-indonesia\lcd-validation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52A33FD-2F09-44AE-BAEB-3A7C28DD3F1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ABD197-7CC8-411D-918D-9660B48571E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7F3B4E45-2D19-4B68-9852-C7B87027CCD1}"/>
   </bookViews>
@@ -1016,6 +1016,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1132,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1160,6 +1163,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1476,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169B3916-394A-4790-A528-B0194DEF6E38}">
   <dimension ref="A1:BM77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2873,11 +2877,11 @@
       <c r="A11" s="10">
         <v>1114</v>
       </c>
-      <c r="B11" s="10">
-        <v>106.753868</v>
+      <c r="B11" s="17">
+        <v>106.753682</v>
       </c>
       <c r="C11" s="10">
-        <v>-6.5521079999999996</v>
+        <v>-6.5524459999999998</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>63</v>

</xml_diff>